<commit_message>
ajustado e testado pela primeira vez
</commit_message>
<xml_diff>
--- a/BASE_KM.xlsx
+++ b/BASE_KM.xlsx
@@ -1,66 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andrew\Desktop\Efetuar_KM\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{562ED24C-D9DD-4ABD-A1E8-20309C0877B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="4890" yWindow="3210" windowWidth="19170" windowHeight="10170" xr2:uid="{96C05B87-CDB6-4313-976E-5A4F82D64B23}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
+    <sheet name="Planilha1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
+  <definedNames/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
-  <si>
-    <t>FILIAL</t>
-  </si>
-  <si>
-    <t>SERIE</t>
-  </si>
-  <si>
-    <t>MANIFESTO</t>
-  </si>
-  <si>
-    <t>KM</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -68,26 +41,167 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="6"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="6"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="6"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="6"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="6"/>
+      </top>
+      <bottom style="thin">
+        <color theme="6"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="6"/>
+      </top>
+      <bottom style="thin">
+        <color theme="6"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+  <cellXfs count="9">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -387,75 +501,185 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{107783A5-CCC7-41CA-BE53-C7C2BD8BDE71}">
-  <dimension ref="A1:D4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="A2" sqref="A2:XFD3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col width="11.42578125" bestFit="1" customWidth="1" min="3" max="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>FILIAL</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>SERIE</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>MANIFESTO</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>KM</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>STATUS</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="B2" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>5</v>
-      </c>
-      <c r="B2">
+      <c r="C2" s="3" t="n">
+        <v>211612</v>
+      </c>
+      <c r="D2" s="4" t="n">
+        <v>665</v>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>MANIFESTO BAIXADO</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C2">
-        <v>21303</v>
-      </c>
-      <c r="D2">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>5</v>
-      </c>
-      <c r="B3">
+      <c r="B3" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C3" s="3" t="n">
+        <v>211617</v>
+      </c>
+      <c r="D3" s="4" t="n">
+        <v>240</v>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>MANIFESTO BAIXADO</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="C3">
-        <v>21302</v>
-      </c>
-      <c r="D3">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>5</v>
-      </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
-      <c r="C4">
-        <v>21304</v>
-      </c>
-      <c r="D4">
-        <v>99</v>
-      </c>
+      <c r="B4" s="6" t="n">
+        <v>2</v>
+      </c>
+      <c r="C4" s="7" t="n">
+        <v>211619</v>
+      </c>
+      <c r="D4" s="8" t="n">
+        <v>555</v>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>MANIFESTO BAIXADO</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n"/>
+      <c r="B5" s="2" t="n"/>
+      <c r="C5" s="3" t="n"/>
+      <c r="D5" s="4" t="n"/>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="n"/>
+      <c r="B6" s="2" t="n"/>
+      <c r="C6" s="3" t="n"/>
+      <c r="D6" s="4" t="n"/>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="n"/>
+      <c r="B7" s="2" t="n"/>
+      <c r="C7" s="3" t="n"/>
+      <c r="D7" s="4" t="n"/>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="n"/>
+      <c r="B8" s="2" t="n"/>
+      <c r="C8" s="3" t="n"/>
+      <c r="D8" s="4" t="n"/>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="n"/>
+      <c r="B9" s="2" t="n"/>
+      <c r="C9" s="3" t="n"/>
+      <c r="D9" s="4" t="n"/>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="n"/>
+      <c r="B10" s="2" t="n"/>
+      <c r="C10" s="3" t="n"/>
+      <c r="D10" s="4" t="n"/>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="n"/>
+      <c r="B11" s="2" t="n"/>
+      <c r="C11" s="3" t="n"/>
+      <c r="D11" s="4" t="n"/>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="n"/>
+      <c r="B12" s="2" t="n"/>
+      <c r="C12" s="3" t="n"/>
+      <c r="D12" s="4" t="n"/>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="n"/>
+      <c r="B13" s="2" t="n"/>
+      <c r="C13" s="3" t="n"/>
+      <c r="D13" s="4" t="n"/>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="n"/>
+      <c r="B14" s="2" t="n"/>
+      <c r="C14" s="3" t="n"/>
+      <c r="D14" s="4" t="n"/>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="n"/>
+      <c r="B15" s="2" t="n"/>
+      <c r="C15" s="3" t="n"/>
+      <c r="D15" s="4" t="n"/>
+    </row>
+    <row r="16">
+      <c r="A16" s="5" t="n"/>
+      <c r="B16" s="6" t="n"/>
+      <c r="C16" s="7" t="n"/>
+      <c r="D16" s="8" t="n"/>
     </row>
   </sheetData>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <conditionalFormatting sqref="C5:C16">
+    <cfRule type="duplicateValues" priority="3" dxfId="0"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C2:C4">
+    <cfRule type="duplicateValues" priority="4" dxfId="0"/>
+  </conditionalFormatting>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.787401575" bottom="0.787401575" header="0.31496062" footer="0.31496062"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
rodado do dia 12.08
</commit_message>
<xml_diff>
--- a/BASE_KM.xlsx
+++ b/BASE_KM.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15390" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" state="visible" r:id="rId1"/>
@@ -33,7 +33,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -61,11 +61,59 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="6"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="6"/>
+      </top>
+      <bottom style="thin">
+        <color theme="6"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="6"/>
+      </top>
+      <bottom style="thin">
+        <color theme="6"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="6"/>
+      </right>
+      <top style="thin">
+        <color theme="6"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="6"/>
+      </right>
+      <top style="thin">
+        <color theme="6"/>
+      </top>
+      <bottom style="thin">
+        <color theme="6"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
@@ -73,54 +121,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -515,10 +534,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E48"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:D24"/>
+      <selection activeCell="A2" sqref="A2:XFD9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -555,15 +574,15 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="n">
-        <v>18</v>
+        <v>2</v>
       </c>
       <c r="C2" s="2" t="n">
-        <v>24233</v>
-      </c>
-      <c r="D2" s="3" t="n">
-        <v>203</v>
-      </c>
-      <c r="E2" t="inlineStr">
+        <v>215489</v>
+      </c>
+      <c r="D2" s="5" t="n">
+        <v>177</v>
+      </c>
+      <c r="E2" s="6" t="inlineStr">
         <is>
           <t>MANIFESTO BAIXADO</t>
         </is>
@@ -574,15 +593,15 @@
         <v>1</v>
       </c>
       <c r="B3" s="2" t="n">
-        <v>18</v>
+        <v>2</v>
       </c>
       <c r="C3" s="2" t="n">
-        <v>24242</v>
-      </c>
-      <c r="D3" s="3" t="n">
-        <v>116</v>
-      </c>
-      <c r="E3" t="inlineStr">
+        <v>215490</v>
+      </c>
+      <c r="D3" s="5" t="n">
+        <v>77</v>
+      </c>
+      <c r="E3" s="6" t="inlineStr">
         <is>
           <t>MANIFESTO BAIXADO</t>
         </is>
@@ -593,15 +612,15 @@
         <v>1</v>
       </c>
       <c r="B4" s="2" t="n">
-        <v>18</v>
+        <v>2</v>
       </c>
       <c r="C4" s="2" t="n">
-        <v>24243</v>
-      </c>
-      <c r="D4" s="3" t="n">
-        <v>143</v>
-      </c>
-      <c r="E4" t="inlineStr">
+        <v>215492</v>
+      </c>
+      <c r="D4" s="5" t="n">
+        <v>119</v>
+      </c>
+      <c r="E4" s="6" t="inlineStr">
         <is>
           <t>MANIFESTO BAIXADO</t>
         </is>
@@ -612,15 +631,15 @@
         <v>1</v>
       </c>
       <c r="B5" s="2" t="n">
-        <v>18</v>
+        <v>2</v>
       </c>
       <c r="C5" s="2" t="n">
-        <v>24226</v>
-      </c>
-      <c r="D5" s="3" t="n">
-        <v>246</v>
-      </c>
-      <c r="E5" t="inlineStr">
+        <v>215493</v>
+      </c>
+      <c r="D5" s="5" t="n">
+        <v>49</v>
+      </c>
+      <c r="E5" s="6" t="inlineStr">
         <is>
           <t>MANIFESTO BAIXADO</t>
         </is>
@@ -631,15 +650,15 @@
         <v>1</v>
       </c>
       <c r="B6" s="2" t="n">
-        <v>18</v>
+        <v>2</v>
       </c>
       <c r="C6" s="2" t="n">
-        <v>24244</v>
-      </c>
-      <c r="D6" s="3" t="n">
-        <v>205</v>
-      </c>
-      <c r="E6" t="inlineStr">
+        <v>215494</v>
+      </c>
+      <c r="D6" s="5" t="n">
+        <v>101</v>
+      </c>
+      <c r="E6" s="6" t="inlineStr">
         <is>
           <t>MANIFESTO BAIXADO</t>
         </is>
@@ -650,15 +669,15 @@
         <v>1</v>
       </c>
       <c r="B7" s="2" t="n">
-        <v>18</v>
+        <v>2</v>
       </c>
       <c r="C7" s="2" t="n">
-        <v>24240</v>
-      </c>
-      <c r="D7" s="3" t="n">
-        <v>348</v>
-      </c>
-      <c r="E7" t="inlineStr">
+        <v>215595</v>
+      </c>
+      <c r="D7" s="5" t="n">
+        <v>270</v>
+      </c>
+      <c r="E7" s="6" t="inlineStr">
         <is>
           <t>MANIFESTO BAIXADO</t>
         </is>
@@ -669,15 +688,15 @@
         <v>1</v>
       </c>
       <c r="B8" s="2" t="n">
-        <v>18</v>
+        <v>2</v>
       </c>
       <c r="C8" s="2" t="n">
-        <v>24238</v>
-      </c>
-      <c r="D8" s="3" t="n">
-        <v>326</v>
-      </c>
-      <c r="E8" t="inlineStr">
+        <v>215620</v>
+      </c>
+      <c r="D8" s="5" t="n">
+        <v>517</v>
+      </c>
+      <c r="E8" s="6" t="inlineStr">
         <is>
           <t>MANIFESTO BAIXADO</t>
         </is>
@@ -688,17 +707,17 @@
         <v>1</v>
       </c>
       <c r="B9" s="2" t="n">
-        <v>18</v>
+        <v>2</v>
       </c>
       <c r="C9" s="2" t="n">
-        <v>24231</v>
-      </c>
-      <c r="D9" s="3" t="n">
-        <v>371</v>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>NAO LOCALIZADO</t>
+        <v>215621</v>
+      </c>
+      <c r="D9" s="5" t="n">
+        <v>230</v>
+      </c>
+      <c r="E9" s="6" t="inlineStr">
+        <is>
+          <t>MANIFESTO BAIXADO</t>
         </is>
       </c>
     </row>
@@ -707,15 +726,15 @@
         <v>1</v>
       </c>
       <c r="B10" s="2" t="n">
-        <v>18</v>
+        <v>2</v>
       </c>
       <c r="C10" s="2" t="n">
-        <v>24229</v>
-      </c>
-      <c r="D10" s="3" t="n">
-        <v>116</v>
-      </c>
-      <c r="E10" t="inlineStr">
+        <v>215623</v>
+      </c>
+      <c r="D10" s="5" t="n">
+        <v>81</v>
+      </c>
+      <c r="E10" s="6" t="inlineStr">
         <is>
           <t>MANIFESTO BAIXADO</t>
         </is>
@@ -726,15 +745,15 @@
         <v>1</v>
       </c>
       <c r="B11" s="2" t="n">
-        <v>18</v>
+        <v>2</v>
       </c>
       <c r="C11" s="2" t="n">
-        <v>24239</v>
-      </c>
-      <c r="D11" s="3" t="n">
-        <v>148</v>
-      </c>
-      <c r="E11" t="inlineStr">
+        <v>215624</v>
+      </c>
+      <c r="D11" s="5" t="n">
+        <v>167</v>
+      </c>
+      <c r="E11" s="6" t="inlineStr">
         <is>
           <t>MANIFESTO BAIXADO</t>
         </is>
@@ -745,15 +764,15 @@
         <v>1</v>
       </c>
       <c r="B12" s="2" t="n">
-        <v>18</v>
+        <v>2</v>
       </c>
       <c r="C12" s="2" t="n">
-        <v>24236</v>
-      </c>
-      <c r="D12" s="3" t="n">
-        <v>254</v>
-      </c>
-      <c r="E12" t="inlineStr">
+        <v>215668</v>
+      </c>
+      <c r="D12" s="5" t="n">
+        <v>270</v>
+      </c>
+      <c r="E12" s="6" t="inlineStr">
         <is>
           <t>MANIFESTO BAIXADO</t>
         </is>
@@ -764,15 +783,15 @@
         <v>1</v>
       </c>
       <c r="B13" s="2" t="n">
-        <v>18</v>
+        <v>2</v>
       </c>
       <c r="C13" s="2" t="n">
-        <v>24235</v>
-      </c>
-      <c r="D13" s="3" t="n">
-        <v>260</v>
-      </c>
-      <c r="E13" t="inlineStr">
+        <v>215735</v>
+      </c>
+      <c r="D13" s="5" t="n">
+        <v>92</v>
+      </c>
+      <c r="E13" s="6" t="inlineStr">
         <is>
           <t>MANIFESTO BAIXADO</t>
         </is>
@@ -783,15 +802,15 @@
         <v>1</v>
       </c>
       <c r="B14" s="2" t="n">
-        <v>18</v>
+        <v>2</v>
       </c>
       <c r="C14" s="2" t="n">
-        <v>24230</v>
-      </c>
-      <c r="D14" s="3" t="n">
-        <v>278</v>
-      </c>
-      <c r="E14" t="inlineStr">
+        <v>215737</v>
+      </c>
+      <c r="D14" s="5" t="n">
+        <v>60</v>
+      </c>
+      <c r="E14" s="6" t="inlineStr">
         <is>
           <t>MANIFESTO BAIXADO</t>
         </is>
@@ -802,15 +821,15 @@
         <v>1</v>
       </c>
       <c r="B15" s="2" t="n">
-        <v>18</v>
+        <v>2</v>
       </c>
       <c r="C15" s="2" t="n">
-        <v>24237</v>
-      </c>
-      <c r="D15" s="3" t="n">
-        <v>87</v>
-      </c>
-      <c r="E15" t="inlineStr">
+        <v>215740</v>
+      </c>
+      <c r="D15" s="5" t="n">
+        <v>151</v>
+      </c>
+      <c r="E15" s="6" t="inlineStr">
         <is>
           <t>MANIFESTO BAIXADO</t>
         </is>
@@ -821,15 +840,15 @@
         <v>1</v>
       </c>
       <c r="B16" s="2" t="n">
-        <v>18</v>
+        <v>2</v>
       </c>
       <c r="C16" s="2" t="n">
-        <v>24241</v>
-      </c>
-      <c r="D16" s="3" t="n">
-        <v>77</v>
-      </c>
-      <c r="E16" t="inlineStr">
+        <v>215742</v>
+      </c>
+      <c r="D16" s="5" t="n">
+        <v>79</v>
+      </c>
+      <c r="E16" s="6" t="inlineStr">
         <is>
           <t>MANIFESTO BAIXADO</t>
         </is>
@@ -840,15 +859,15 @@
         <v>1</v>
       </c>
       <c r="B17" s="2" t="n">
-        <v>18</v>
+        <v>2</v>
       </c>
       <c r="C17" s="2" t="n">
-        <v>24232</v>
-      </c>
-      <c r="D17" s="3" t="n">
-        <v>140</v>
-      </c>
-      <c r="E17" t="inlineStr">
+        <v>215744</v>
+      </c>
+      <c r="D17" s="5" t="n">
+        <v>150</v>
+      </c>
+      <c r="E17" s="6" t="inlineStr">
         <is>
           <t>MANIFESTO BAIXADO</t>
         </is>
@@ -859,15 +878,15 @@
         <v>1</v>
       </c>
       <c r="B18" s="2" t="n">
-        <v>18</v>
+        <v>2</v>
       </c>
       <c r="C18" s="2" t="n">
-        <v>24234</v>
-      </c>
-      <c r="D18" s="3" t="n">
-        <v>86</v>
-      </c>
-      <c r="E18" t="inlineStr">
+        <v>215746</v>
+      </c>
+      <c r="D18" s="5" t="n">
+        <v>110</v>
+      </c>
+      <c r="E18" s="6" t="inlineStr">
         <is>
           <t>MANIFESTO BAIXADO</t>
         </is>
@@ -878,271 +897,45 @@
         <v>1</v>
       </c>
       <c r="B19" s="2" t="n">
-        <v>18</v>
+        <v>2</v>
       </c>
       <c r="C19" s="2" t="n">
-        <v>24223</v>
-      </c>
-      <c r="D19" s="3" t="n">
-        <v>122</v>
-      </c>
-      <c r="E19" t="inlineStr">
+        <v>215491</v>
+      </c>
+      <c r="D19" s="5" t="n">
+        <v>276</v>
+      </c>
+      <c r="E19" s="6" t="inlineStr">
         <is>
           <t>MANIFESTO BAIXADO</t>
         </is>
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="B20" s="2" t="n">
-        <v>18</v>
-      </c>
-      <c r="C20" s="2" t="n">
-        <v>24224</v>
-      </c>
-      <c r="D20" s="3" t="n">
-        <v>129</v>
-      </c>
-      <c r="E20" t="inlineStr">
-        <is>
-          <t>MANIFESTO BAIXADO</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="B21" s="2" t="n">
-        <v>18</v>
-      </c>
-      <c r="C21" s="2" t="n">
-        <v>24227</v>
-      </c>
-      <c r="D21" s="3" t="n">
-        <v>232</v>
-      </c>
-      <c r="E21" t="inlineStr">
-        <is>
-          <t>MANIFESTO BAIXADO</t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="B22" s="2" t="n">
-        <v>18</v>
-      </c>
-      <c r="C22" s="2" t="n">
-        <v>24222</v>
-      </c>
-      <c r="D22" s="3" t="n">
-        <v>80</v>
-      </c>
-      <c r="E22" t="inlineStr">
-        <is>
-          <t>MANIFESTO BAIXADO</t>
-        </is>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="B23" s="2" t="n">
-        <v>18</v>
-      </c>
-      <c r="C23" s="2" t="n">
-        <v>24228</v>
-      </c>
-      <c r="D23" s="3" t="n">
-        <v>101</v>
-      </c>
-      <c r="E23" t="inlineStr">
-        <is>
-          <t>MANIFESTO BAIXADO</t>
-        </is>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="B24" s="2" t="n">
-        <v>18</v>
-      </c>
-      <c r="C24" s="2" t="n">
-        <v>24225</v>
-      </c>
-      <c r="D24" s="3" t="n">
-        <v>109</v>
-      </c>
-      <c r="E24" t="inlineStr">
-        <is>
-          <t>MANIFESTO BAIXADO</t>
-        </is>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" s="1" t="n"/>
-      <c r="B25" s="2" t="n"/>
-      <c r="C25" s="2" t="n"/>
-      <c r="D25" s="3" t="n"/>
-    </row>
-    <row r="26">
-      <c r="A26" s="1" t="n"/>
-      <c r="B26" s="2" t="n"/>
-      <c r="C26" s="2" t="n"/>
-      <c r="D26" s="3" t="n"/>
-    </row>
-    <row r="27">
-      <c r="A27" s="1" t="n"/>
-      <c r="B27" s="2" t="n"/>
-      <c r="C27" s="2" t="n"/>
-      <c r="D27" s="3" t="n"/>
-    </row>
-    <row r="28">
-      <c r="A28" s="1" t="n"/>
-      <c r="B28" s="2" t="n"/>
-      <c r="C28" s="2" t="n"/>
-      <c r="D28" s="3" t="n"/>
-    </row>
-    <row r="29">
-      <c r="A29" s="1" t="n"/>
-      <c r="B29" s="2" t="n"/>
-      <c r="C29" s="2" t="n"/>
-      <c r="D29" s="3" t="n"/>
-    </row>
-    <row r="30">
-      <c r="A30" s="1" t="n"/>
-      <c r="B30" s="2" t="n"/>
-      <c r="C30" s="2" t="n"/>
-      <c r="D30" s="3" t="n"/>
-    </row>
-    <row r="31">
-      <c r="A31" s="1" t="n"/>
-      <c r="B31" s="2" t="n"/>
-      <c r="C31" s="2" t="n"/>
-      <c r="D31" s="3" t="n"/>
-    </row>
-    <row r="32">
-      <c r="A32" s="1" t="n"/>
-      <c r="B32" s="2" t="n"/>
-      <c r="C32" s="2" t="n"/>
-      <c r="D32" s="3" t="n"/>
-    </row>
-    <row r="33">
-      <c r="A33" s="1" t="n"/>
-      <c r="B33" s="2" t="n"/>
-      <c r="C33" s="2" t="n"/>
-      <c r="D33" s="3" t="n"/>
-    </row>
-    <row r="34">
-      <c r="A34" s="1" t="n"/>
-      <c r="B34" s="2" t="n"/>
-      <c r="C34" s="2" t="n"/>
-      <c r="D34" s="3" t="n"/>
-    </row>
-    <row r="35">
-      <c r="A35" s="1" t="n"/>
-      <c r="B35" s="2" t="n"/>
-      <c r="C35" s="2" t="n"/>
-      <c r="D35" s="3" t="n"/>
-    </row>
-    <row r="36">
-      <c r="A36" s="1" t="n"/>
-      <c r="B36" s="2" t="n"/>
-      <c r="C36" s="2" t="n"/>
-      <c r="D36" s="3" t="n"/>
-    </row>
-    <row r="37">
-      <c r="A37" s="1" t="n"/>
-      <c r="B37" s="2" t="n"/>
-      <c r="C37" s="2" t="n"/>
-      <c r="D37" s="3" t="n"/>
-    </row>
-    <row r="38">
-      <c r="A38" s="1" t="n"/>
-      <c r="B38" s="2" t="n"/>
-      <c r="C38" s="2" t="n"/>
-      <c r="D38" s="3" t="n"/>
-    </row>
-    <row r="39">
-      <c r="A39" s="1" t="n"/>
-      <c r="B39" s="2" t="n"/>
-      <c r="C39" s="2" t="n"/>
-      <c r="D39" s="3" t="n"/>
-    </row>
-    <row r="40">
-      <c r="A40" s="1" t="n"/>
-      <c r="B40" s="2" t="n"/>
-      <c r="C40" s="2" t="n"/>
-      <c r="D40" s="3" t="n"/>
-    </row>
-    <row r="41">
-      <c r="A41" s="1" t="n"/>
-      <c r="B41" s="2" t="n"/>
-      <c r="C41" s="2" t="n"/>
-      <c r="D41" s="3" t="n"/>
-    </row>
-    <row r="42">
-      <c r="A42" s="1" t="n"/>
-      <c r="B42" s="2" t="n"/>
-      <c r="C42" s="2" t="n"/>
-      <c r="D42" s="3" t="n"/>
-    </row>
-    <row r="43">
-      <c r="A43" s="1" t="n"/>
-      <c r="B43" s="2" t="n"/>
-      <c r="C43" s="2" t="n"/>
-      <c r="D43" s="3" t="n"/>
-    </row>
-    <row r="44">
-      <c r="A44" s="1" t="n"/>
-      <c r="B44" s="2" t="n"/>
-      <c r="C44" s="2" t="n"/>
-      <c r="D44" s="3" t="n"/>
-    </row>
-    <row r="45">
-      <c r="A45" s="1" t="n"/>
-      <c r="B45" s="2" t="n"/>
-      <c r="C45" s="2" t="n"/>
-      <c r="D45" s="3" t="n"/>
-    </row>
-    <row r="46">
-      <c r="A46" s="1" t="n"/>
-      <c r="B46" s="2" t="n"/>
-      <c r="C46" s="2" t="n"/>
-      <c r="D46" s="3" t="n"/>
-    </row>
-    <row r="47">
-      <c r="A47" s="1" t="n"/>
-      <c r="B47" s="2" t="n"/>
-      <c r="C47" s="2" t="n"/>
-      <c r="D47" s="3" t="n"/>
-    </row>
-    <row r="48">
-      <c r="A48" s="1" t="n"/>
-      <c r="B48" s="2" t="n"/>
-      <c r="C48" s="2" t="n"/>
-      <c r="D48" s="3" t="n"/>
+      <c r="A20" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="B20" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="C20" s="4" t="n">
+        <v>215276</v>
+      </c>
+      <c r="D20" s="7" t="n">
+        <v>217</v>
+      </c>
+      <c r="E20" s="8" t="inlineStr">
+        <is>
+          <t>MANIFESTO BAIXADO</t>
+        </is>
+      </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C25:C48">
-    <cfRule type="duplicateValues" priority="7" dxfId="0"/>
+  <conditionalFormatting sqref="C2:C20">
+    <cfRule type="duplicateValues" priority="3" dxfId="0"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D25:D48">
-    <cfRule type="duplicateValues" priority="8" dxfId="0"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C2:C24">
-    <cfRule type="duplicateValues" priority="1" dxfId="0"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D2:D24">
-    <cfRule type="duplicateValues" priority="2" dxfId="0"/>
+  <conditionalFormatting sqref="D2:D20">
+    <cfRule type="duplicateValues" priority="4" dxfId="0"/>
   </conditionalFormatting>
   <pageMargins left="0.511811024" right="0.511811024" top="0.787401575" bottom="0.787401575" header="0.31496062" footer="0.31496062"/>
 </worksheet>

</xml_diff>

<commit_message>
feito clicks direto nos botoes em vez de ir andando usando o teclado
</commit_message>
<xml_diff>
--- a/BASE_KM.xlsx
+++ b/BASE_KM.xlsx
@@ -3,20 +3,29 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15390" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="191029" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+  </numFmts>
+  <fonts count="2">
+    <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -110,10 +119,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  <cellStyleXfs count="2">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
@@ -135,11 +145,35 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Vírgula" xfId="1" builtinId="3"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="4">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -537,7 +571,7 @@
   <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD9"/>
+      <selection activeCell="A2" sqref="A2:D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -577,10 +611,10 @@
         <v>2</v>
       </c>
       <c r="C2" s="2" t="n">
-        <v>215489</v>
-      </c>
-      <c r="D2" s="5" t="n">
-        <v>177</v>
+        <v>215855</v>
+      </c>
+      <c r="D2" s="9" t="n">
+        <v>24</v>
       </c>
       <c r="E2" s="6" t="inlineStr">
         <is>
@@ -596,10 +630,10 @@
         <v>2</v>
       </c>
       <c r="C3" s="2" t="n">
-        <v>215490</v>
-      </c>
-      <c r="D3" s="5" t="n">
-        <v>77</v>
+        <v>215857</v>
+      </c>
+      <c r="D3" s="9" t="n">
+        <v>24</v>
       </c>
       <c r="E3" s="6" t="inlineStr">
         <is>
@@ -615,10 +649,10 @@
         <v>2</v>
       </c>
       <c r="C4" s="2" t="n">
-        <v>215492</v>
-      </c>
-      <c r="D4" s="5" t="n">
-        <v>119</v>
+        <v>215899</v>
+      </c>
+      <c r="D4" s="9" t="n">
+        <v>102</v>
       </c>
       <c r="E4" s="6" t="inlineStr">
         <is>
@@ -634,10 +668,10 @@
         <v>2</v>
       </c>
       <c r="C5" s="2" t="n">
-        <v>215493</v>
-      </c>
-      <c r="D5" s="5" t="n">
-        <v>49</v>
+        <v>215854</v>
+      </c>
+      <c r="D5" s="9" t="n">
+        <v>669</v>
       </c>
       <c r="E5" s="6" t="inlineStr">
         <is>
@@ -653,10 +687,10 @@
         <v>2</v>
       </c>
       <c r="C6" s="2" t="n">
-        <v>215494</v>
-      </c>
-      <c r="D6" s="5" t="n">
-        <v>101</v>
+        <v>215900</v>
+      </c>
+      <c r="D6" s="9" t="n">
+        <v>3</v>
       </c>
       <c r="E6" s="6" t="inlineStr">
         <is>
@@ -672,10 +706,10 @@
         <v>2</v>
       </c>
       <c r="C7" s="2" t="n">
-        <v>215595</v>
-      </c>
-      <c r="D7" s="5" t="n">
-        <v>270</v>
+        <v>215852</v>
+      </c>
+      <c r="D7" s="9" t="n">
+        <v>669</v>
       </c>
       <c r="E7" s="6" t="inlineStr">
         <is>
@@ -691,10 +725,10 @@
         <v>2</v>
       </c>
       <c r="C8" s="2" t="n">
-        <v>215620</v>
-      </c>
-      <c r="D8" s="5" t="n">
-        <v>517</v>
+        <v>215886</v>
+      </c>
+      <c r="D8" s="9" t="n">
+        <v>197</v>
       </c>
       <c r="E8" s="6" t="inlineStr">
         <is>
@@ -710,10 +744,10 @@
         <v>2</v>
       </c>
       <c r="C9" s="2" t="n">
-        <v>215621</v>
-      </c>
-      <c r="D9" s="5" t="n">
-        <v>230</v>
+        <v>215853</v>
+      </c>
+      <c r="D9" s="9" t="n">
+        <v>97</v>
       </c>
       <c r="E9" s="6" t="inlineStr">
         <is>
@@ -729,10 +763,10 @@
         <v>2</v>
       </c>
       <c r="C10" s="2" t="n">
-        <v>215623</v>
-      </c>
-      <c r="D10" s="5" t="n">
-        <v>81</v>
+        <v>215862</v>
+      </c>
+      <c r="D10" s="9" t="n">
+        <v>265</v>
       </c>
       <c r="E10" s="6" t="inlineStr">
         <is>
@@ -748,10 +782,10 @@
         <v>2</v>
       </c>
       <c r="C11" s="2" t="n">
-        <v>215624</v>
-      </c>
-      <c r="D11" s="5" t="n">
-        <v>167</v>
+        <v>215865</v>
+      </c>
+      <c r="D11" s="9" t="n">
+        <v>223</v>
       </c>
       <c r="E11" s="6" t="inlineStr">
         <is>
@@ -767,10 +801,10 @@
         <v>2</v>
       </c>
       <c r="C12" s="2" t="n">
-        <v>215668</v>
-      </c>
-      <c r="D12" s="5" t="n">
-        <v>270</v>
+        <v>215867</v>
+      </c>
+      <c r="D12" s="9" t="n">
+        <v>194</v>
       </c>
       <c r="E12" s="6" t="inlineStr">
         <is>
@@ -786,10 +820,10 @@
         <v>2</v>
       </c>
       <c r="C13" s="2" t="n">
-        <v>215735</v>
-      </c>
-      <c r="D13" s="5" t="n">
-        <v>92</v>
+        <v>215868</v>
+      </c>
+      <c r="D13" s="9" t="n">
+        <v>234</v>
       </c>
       <c r="E13" s="6" t="inlineStr">
         <is>
@@ -798,144 +832,66 @@
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="B14" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="C14" s="2" t="n">
-        <v>215737</v>
-      </c>
-      <c r="D14" s="5" t="n">
-        <v>60</v>
-      </c>
-      <c r="E14" s="6" t="inlineStr">
-        <is>
-          <t>MANIFESTO BAIXADO</t>
-        </is>
-      </c>
+      <c r="A14" s="1" t="n"/>
+      <c r="B14" s="2" t="n"/>
+      <c r="C14" s="2" t="n"/>
+      <c r="D14" s="5" t="n"/>
+      <c r="E14" s="6" t="n"/>
     </row>
     <row r="15">
-      <c r="A15" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="B15" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="C15" s="2" t="n">
-        <v>215740</v>
-      </c>
-      <c r="D15" s="5" t="n">
-        <v>151</v>
-      </c>
-      <c r="E15" s="6" t="inlineStr">
-        <is>
-          <t>MANIFESTO BAIXADO</t>
-        </is>
-      </c>
+      <c r="A15" s="1" t="n"/>
+      <c r="B15" s="2" t="n"/>
+      <c r="C15" s="2" t="n"/>
+      <c r="D15" s="5" t="n"/>
+      <c r="E15" s="6" t="n"/>
     </row>
     <row r="16">
-      <c r="A16" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="B16" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="C16" s="2" t="n">
-        <v>215742</v>
-      </c>
-      <c r="D16" s="5" t="n">
-        <v>79</v>
-      </c>
-      <c r="E16" s="6" t="inlineStr">
-        <is>
-          <t>MANIFESTO BAIXADO</t>
-        </is>
-      </c>
+      <c r="A16" s="1" t="n"/>
+      <c r="B16" s="2" t="n"/>
+      <c r="C16" s="2" t="n"/>
+      <c r="D16" s="5" t="n"/>
+      <c r="E16" s="6" t="n"/>
     </row>
     <row r="17">
-      <c r="A17" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="B17" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="C17" s="2" t="n">
-        <v>215744</v>
-      </c>
-      <c r="D17" s="5" t="n">
-        <v>150</v>
-      </c>
-      <c r="E17" s="6" t="inlineStr">
-        <is>
-          <t>MANIFESTO BAIXADO</t>
-        </is>
-      </c>
+      <c r="A17" s="1" t="n"/>
+      <c r="B17" s="2" t="n"/>
+      <c r="C17" s="2" t="n"/>
+      <c r="D17" s="5" t="n"/>
+      <c r="E17" s="6" t="n"/>
     </row>
     <row r="18">
-      <c r="A18" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="B18" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="C18" s="2" t="n">
-        <v>215746</v>
-      </c>
-      <c r="D18" s="5" t="n">
-        <v>110</v>
-      </c>
-      <c r="E18" s="6" t="inlineStr">
-        <is>
-          <t>MANIFESTO BAIXADO</t>
-        </is>
-      </c>
+      <c r="A18" s="1" t="n"/>
+      <c r="B18" s="2" t="n"/>
+      <c r="C18" s="2" t="n"/>
+      <c r="D18" s="5" t="n"/>
+      <c r="E18" s="6" t="n"/>
     </row>
     <row r="19">
-      <c r="A19" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="B19" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="C19" s="2" t="n">
-        <v>215491</v>
-      </c>
-      <c r="D19" s="5" t="n">
-        <v>276</v>
-      </c>
-      <c r="E19" s="6" t="inlineStr">
-        <is>
-          <t>MANIFESTO BAIXADO</t>
-        </is>
-      </c>
+      <c r="A19" s="1" t="n"/>
+      <c r="B19" s="2" t="n"/>
+      <c r="C19" s="2" t="n"/>
+      <c r="D19" s="5" t="n"/>
+      <c r="E19" s="6" t="n"/>
     </row>
     <row r="20">
-      <c r="A20" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="B20" s="4" t="n">
-        <v>2</v>
-      </c>
-      <c r="C20" s="4" t="n">
-        <v>215276</v>
-      </c>
-      <c r="D20" s="7" t="n">
-        <v>217</v>
-      </c>
-      <c r="E20" s="8" t="inlineStr">
-        <is>
-          <t>MANIFESTO BAIXADO</t>
-        </is>
-      </c>
+      <c r="A20" s="3" t="n"/>
+      <c r="B20" s="4" t="n"/>
+      <c r="C20" s="4" t="n"/>
+      <c r="D20" s="7" t="n"/>
+      <c r="E20" s="8" t="n"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C2:C20">
-    <cfRule type="duplicateValues" priority="3" dxfId="0"/>
+  <conditionalFormatting sqref="C14:C20">
+    <cfRule type="duplicateValues" priority="5" dxfId="0"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D2:D20">
-    <cfRule type="duplicateValues" priority="4" dxfId="0"/>
+  <conditionalFormatting sqref="D14:D20">
+    <cfRule type="duplicateValues" priority="6" dxfId="0"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C2:C13">
+    <cfRule type="duplicateValues" priority="1" dxfId="0"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D2:D13">
+    <cfRule type="duplicateValues" priority="2" dxfId="0"/>
   </conditionalFormatting>
   <pageMargins left="0.511811024" right="0.511811024" top="0.787401575" bottom="0.787401575" header="0.31496062" footer="0.31496062"/>
 </worksheet>

</xml_diff>